<commit_message>
Trial 2 datasheet finalizations.
</commit_message>
<xml_diff>
--- a/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/datasheets/flight_T2_datasheet.xlsx
+++ b/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/datasheets/flight_T2_datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/SBB-dispersal/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8B4777E7-5842-A44D-8D6E-9056BFF0D426}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2C74FD15-0907-4748-9DFF-B536C0D6A054}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16160"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -99,12 +99,18 @@
   <si>
     <t>Gainesville</t>
   </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>escaped</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,6 +255,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -436,7 +449,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -566,6 +579,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -611,11 +646,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -971,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P297"/>
+  <dimension ref="A1:Q298"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J287" sqref="J287"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="132" workbookViewId="0">
+      <selection activeCell="Q125" sqref="Q125:Q137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -994,7 +1035,7 @@
     <col min="13" max="13" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.1640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6" style="1" customWidth="1"/>
+    <col min="16" max="16" width="6" style="4" customWidth="1"/>
     <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1044,7 +1085,7 @@
       <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1074,7 +1115,7 @@
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="P2" s="6"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
@@ -1102,7 +1143,7 @@
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="P3" s="6"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -1130,7 +1171,7 @@
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="P4" s="6"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -1158,7 +1199,7 @@
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
+      <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
@@ -1186,7 +1227,7 @@
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="P6" s="6"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -1214,7 +1255,7 @@
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="P7" s="6"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -1242,13 +1283,15 @@
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="P8" s="6"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>32</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1270,7 +1313,7 @@
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -1298,7 +1341,7 @@
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -1326,7 +1369,7 @@
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+      <c r="P11" s="6"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -1354,7 +1397,7 @@
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -1382,7 +1425,7 @@
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
+      <c r="P13" s="6"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
@@ -1410,7 +1453,7 @@
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
+      <c r="P14" s="6"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -1438,7 +1481,7 @@
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
+      <c r="P15" s="6"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -1466,7 +1509,7 @@
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="P16" s="6"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
@@ -1494,7 +1537,7 @@
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+      <c r="P17" s="6"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
@@ -1522,7 +1565,7 @@
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
+      <c r="P18" s="6"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
@@ -1550,7 +1593,7 @@
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
+      <c r="P19" s="6"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -1578,7 +1621,7 @@
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
+      <c r="P20" s="6"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -1606,7 +1649,7 @@
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
+      <c r="P21" s="6"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
@@ -1634,7 +1677,7 @@
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
+      <c r="P22" s="6"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
@@ -1662,7 +1705,7 @@
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
+      <c r="P23" s="6"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
@@ -1690,7 +1733,7 @@
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
+      <c r="P24" s="6"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
@@ -1718,7 +1761,7 @@
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
+      <c r="P25" s="6"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
@@ -1746,7 +1789,7 @@
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
+      <c r="P26" s="6"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
@@ -1774,7 +1817,7 @@
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
+      <c r="P27" s="6"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
@@ -1802,7 +1845,7 @@
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
+      <c r="P28" s="6"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
@@ -1830,7 +1873,7 @@
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
+      <c r="P29" s="6"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
@@ -1858,7 +1901,7 @@
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
+      <c r="P30" s="6"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
@@ -1886,7 +1929,7 @@
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
+      <c r="P31" s="6"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
@@ -1914,7 +1957,7 @@
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
+      <c r="P32" s="6"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
@@ -1942,7 +1985,7 @@
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
+      <c r="P33" s="6"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
@@ -1990,7 +2033,7 @@
       <c r="O34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P34" s="3" t="s">
+      <c r="P34" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2020,7 +2063,7 @@
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
+      <c r="P35" s="6"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
@@ -2048,7 +2091,7 @@
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
+      <c r="P36" s="6"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
@@ -2076,7 +2119,7 @@
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
+      <c r="P37" s="6"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
@@ -2104,7 +2147,7 @@
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
+      <c r="P38" s="6"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
@@ -2132,7 +2175,7 @@
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
+      <c r="P39" s="6"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
@@ -2160,7 +2203,7 @@
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
+      <c r="P40" s="6"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
@@ -2188,7 +2231,7 @@
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
+      <c r="P41" s="6"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
@@ -2216,7 +2259,7 @@
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
+      <c r="P42" s="6"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
@@ -2244,7 +2287,7 @@
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
+      <c r="P43" s="6"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
@@ -2272,7 +2315,7 @@
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
+      <c r="P44" s="6"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
@@ -2300,7 +2343,7 @@
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
+      <c r="P45" s="6"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
@@ -2328,7 +2371,7 @@
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
+      <c r="P46" s="6"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
@@ -2356,7 +2399,7 @@
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
+      <c r="P47" s="6"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
@@ -2384,7 +2427,7 @@
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
+      <c r="P48" s="6"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
@@ -2412,7 +2455,7 @@
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
+      <c r="P49" s="6"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
@@ -2440,7 +2483,7 @@
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
+      <c r="P50" s="6"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
@@ -2468,7 +2511,7 @@
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
-      <c r="P51" s="2"/>
+      <c r="P51" s="6"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
@@ -2496,7 +2539,7 @@
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
+      <c r="P52" s="6"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
@@ -2524,13 +2567,15 @@
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
+      <c r="P53" s="6"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>256</v>
       </c>
-      <c r="B54" s="2"/>
+      <c r="B54" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2552,7 +2597,7 @@
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
-      <c r="P54" s="2"/>
+      <c r="P54" s="6"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
@@ -2580,7 +2625,7 @@
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
-      <c r="P55" s="2"/>
+      <c r="P55" s="6"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
@@ -2608,7 +2653,7 @@
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
+      <c r="P56" s="6"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
@@ -2636,7 +2681,7 @@
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
+      <c r="P57" s="6"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
@@ -2664,7 +2709,7 @@
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
-      <c r="P58" s="2"/>
+      <c r="P58" s="6"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
@@ -2692,7 +2737,7 @@
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
+      <c r="P59" s="6"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
@@ -2720,7 +2765,7 @@
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
-      <c r="P60" s="2"/>
+      <c r="P60" s="6"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
@@ -2748,7 +2793,7 @@
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
-      <c r="P61" s="2"/>
+      <c r="P61" s="6"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
@@ -2776,7 +2821,7 @@
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
-      <c r="P62" s="2"/>
+      <c r="P62" s="6"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
@@ -2804,13 +2849,15 @@
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
-      <c r="P63" s="2"/>
+      <c r="P63" s="6"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>102</v>
       </c>
-      <c r="B64" s="2"/>
+      <c r="B64" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -2832,7 +2879,9 @@
       </c>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
-      <c r="P64" s="2"/>
+      <c r="P64" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
@@ -2860,7 +2909,7 @@
       </c>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
-      <c r="P65" s="2"/>
+      <c r="P65" s="6"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
@@ -2888,7 +2937,7 @@
       </c>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
-      <c r="P66" s="2"/>
+      <c r="P66" s="6"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
@@ -2936,7 +2985,7 @@
       <c r="O67" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P67" s="3" t="s">
+      <c r="P67" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2966,13 +3015,15 @@
       </c>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
-      <c r="P68" s="2"/>
+      <c r="P68" s="6"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>96</v>
       </c>
-      <c r="B69" s="2"/>
+      <c r="B69" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -2994,7 +3045,7 @@
       </c>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
-      <c r="P69" s="2"/>
+      <c r="P69" s="6"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
@@ -3022,7 +3073,7 @@
       </c>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
-      <c r="P70" s="2"/>
+      <c r="P70" s="6"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
@@ -3050,7 +3101,7 @@
       </c>
       <c r="N71" s="2"/>
       <c r="O71" s="2"/>
-      <c r="P71" s="2"/>
+      <c r="P71" s="6"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
@@ -3078,7 +3129,7 @@
       </c>
       <c r="N72" s="2"/>
       <c r="O72" s="2"/>
-      <c r="P72" s="2"/>
+      <c r="P72" s="6"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
@@ -3106,7 +3157,7 @@
       </c>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
-      <c r="P73" s="2"/>
+      <c r="P73" s="6"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
@@ -3134,7 +3185,7 @@
       </c>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
-      <c r="P74" s="2"/>
+      <c r="P74" s="6"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
@@ -3162,7 +3213,7 @@
       </c>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
-      <c r="P75" s="2"/>
+      <c r="P75" s="6"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
@@ -3190,7 +3241,7 @@
       </c>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
-      <c r="P76" s="2"/>
+      <c r="P76" s="6"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
@@ -3218,7 +3269,7 @@
       </c>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
-      <c r="P77" s="2"/>
+      <c r="P77" s="6"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
@@ -3246,7 +3297,7 @@
       </c>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
-      <c r="P78" s="2"/>
+      <c r="P78" s="6"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
@@ -3274,7 +3325,7 @@
       </c>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
-      <c r="P79" s="2"/>
+      <c r="P79" s="6"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
@@ -3302,7 +3353,7 @@
       </c>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
-      <c r="P80" s="2"/>
+      <c r="P80" s="6"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
@@ -3330,7 +3381,7 @@
       </c>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
-      <c r="P81" s="2"/>
+      <c r="P81" s="6"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
@@ -3358,7 +3409,7 @@
       </c>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
-      <c r="P82" s="2"/>
+      <c r="P82" s="6"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
@@ -3386,7 +3437,7 @@
       </c>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
-      <c r="P83" s="2"/>
+      <c r="P83" s="6"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
@@ -3414,7 +3465,7 @@
       </c>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
-      <c r="P84" s="2"/>
+      <c r="P84" s="6"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
@@ -3442,7 +3493,7 @@
       </c>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
-      <c r="P85" s="2"/>
+      <c r="P85" s="6"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
@@ -3470,7 +3521,7 @@
       </c>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
-      <c r="P86" s="2"/>
+      <c r="P86" s="6"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
@@ -3498,7 +3549,7 @@
       </c>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
-      <c r="P87" s="2"/>
+      <c r="P87" s="6"/>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
@@ -3526,7 +3577,7 @@
       </c>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
-      <c r="P88" s="2"/>
+      <c r="P88" s="6"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
@@ -3554,13 +3605,15 @@
       </c>
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
-      <c r="P89" s="2"/>
+      <c r="P89" s="6"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>2</v>
       </c>
-      <c r="B90" s="2"/>
+      <c r="B90" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -3582,7 +3635,7 @@
       </c>
       <c r="N90" s="2"/>
       <c r="O90" s="2"/>
-      <c r="P90" s="2"/>
+      <c r="P90" s="6"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
@@ -3610,7 +3663,7 @@
       </c>
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
-      <c r="P91" s="2"/>
+      <c r="P91" s="6"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
@@ -3638,7 +3691,7 @@
       </c>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
-      <c r="P92" s="2"/>
+      <c r="P92" s="6"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
@@ -3666,13 +3719,15 @@
       </c>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
-      <c r="P93" s="2"/>
+      <c r="P93" s="6"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>244</v>
       </c>
-      <c r="B94" s="2"/>
+      <c r="B94" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -3694,7 +3749,7 @@
       </c>
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
-      <c r="P94" s="2"/>
+      <c r="P94" s="6"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
@@ -3722,7 +3777,7 @@
       </c>
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
-      <c r="P95" s="2"/>
+      <c r="P95" s="6"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
@@ -3750,7 +3805,7 @@
       </c>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
-      <c r="P96" s="2"/>
+      <c r="P96" s="6"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
@@ -3778,7 +3833,7 @@
       </c>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
-      <c r="P97" s="2"/>
+      <c r="P97" s="6"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
@@ -3806,13 +3861,15 @@
       </c>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
-      <c r="P98" s="2"/>
+      <c r="P98" s="6"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>393</v>
       </c>
-      <c r="B99" s="2"/>
+      <c r="B99" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -3834,7 +3891,7 @@
       </c>
       <c r="N99" s="2"/>
       <c r="O99" s="2"/>
-      <c r="P99" s="2"/>
+      <c r="P99" s="6"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
@@ -3882,7 +3939,7 @@
       <c r="O100" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P100" s="3" t="s">
+      <c r="P100" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3912,7 +3969,7 @@
       </c>
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
-      <c r="P101" s="2"/>
+      <c r="P101" s="6"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
@@ -3940,7 +3997,7 @@
       </c>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
-      <c r="P102" s="2"/>
+      <c r="P102" s="6"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
@@ -3968,7 +4025,7 @@
       </c>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
-      <c r="P103" s="2"/>
+      <c r="P103" s="6"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
@@ -3996,7 +4053,7 @@
       </c>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
-      <c r="P104" s="2"/>
+      <c r="P104" s="6"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
@@ -4024,7 +4081,7 @@
       </c>
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
-      <c r="P105" s="2"/>
+      <c r="P105" s="6"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
@@ -4052,7 +4109,7 @@
       </c>
       <c r="N106" s="2"/>
       <c r="O106" s="2"/>
-      <c r="P106" s="2"/>
+      <c r="P106" s="6"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
@@ -4080,7 +4137,7 @@
       </c>
       <c r="N107" s="2"/>
       <c r="O107" s="2"/>
-      <c r="P107" s="2"/>
+      <c r="P107" s="6"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
@@ -4108,7 +4165,7 @@
       </c>
       <c r="N108" s="2"/>
       <c r="O108" s="2"/>
-      <c r="P108" s="2"/>
+      <c r="P108" s="6"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
@@ -4136,7 +4193,7 @@
       </c>
       <c r="N109" s="2"/>
       <c r="O109" s="2"/>
-      <c r="P109" s="2"/>
+      <c r="P109" s="6"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
@@ -4164,7 +4221,7 @@
       </c>
       <c r="N110" s="2"/>
       <c r="O110" s="2"/>
-      <c r="P110" s="2"/>
+      <c r="P110" s="6"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
@@ -4192,7 +4249,7 @@
       </c>
       <c r="N111" s="2"/>
       <c r="O111" s="2"/>
-      <c r="P111" s="2"/>
+      <c r="P111" s="6"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
@@ -4220,7 +4277,7 @@
       </c>
       <c r="N112" s="2"/>
       <c r="O112" s="2"/>
-      <c r="P112" s="2"/>
+      <c r="P112" s="6"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
@@ -4248,7 +4305,7 @@
       </c>
       <c r="N113" s="2"/>
       <c r="O113" s="2"/>
-      <c r="P113" s="2"/>
+      <c r="P113" s="6"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
@@ -4276,7 +4333,7 @@
       </c>
       <c r="N114" s="2"/>
       <c r="O114" s="2"/>
-      <c r="P114" s="2"/>
+      <c r="P114" s="6"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
@@ -4304,13 +4361,15 @@
       </c>
       <c r="N115" s="2"/>
       <c r="O115" s="2"/>
-      <c r="P115" s="2"/>
+      <c r="P115" s="6"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>347</v>
       </c>
-      <c r="B116" s="2"/>
+      <c r="B116" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
@@ -4332,7 +4391,7 @@
       </c>
       <c r="N116" s="2"/>
       <c r="O116" s="2"/>
-      <c r="P116" s="2"/>
+      <c r="P116" s="6"/>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
@@ -4360,7 +4419,7 @@
       </c>
       <c r="N117" s="2"/>
       <c r="O117" s="2"/>
-      <c r="P117" s="2"/>
+      <c r="P117" s="6"/>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
@@ -4388,7 +4447,7 @@
       </c>
       <c r="N118" s="2"/>
       <c r="O118" s="2"/>
-      <c r="P118" s="2"/>
+      <c r="P118" s="6"/>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
@@ -4416,7 +4475,7 @@
       </c>
       <c r="N119" s="2"/>
       <c r="O119" s="2"/>
-      <c r="P119" s="2"/>
+      <c r="P119" s="6"/>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
@@ -4444,7 +4503,7 @@
       </c>
       <c r="N120" s="2"/>
       <c r="O120" s="2"/>
-      <c r="P120" s="2"/>
+      <c r="P120" s="6"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
@@ -4472,7 +4531,7 @@
       </c>
       <c r="N121" s="2"/>
       <c r="O121" s="2"/>
-      <c r="P121" s="2"/>
+      <c r="P121" s="6"/>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
@@ -4500,7 +4559,7 @@
       </c>
       <c r="N122" s="2"/>
       <c r="O122" s="2"/>
-      <c r="P122" s="2"/>
+      <c r="P122" s="6"/>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
@@ -4528,7 +4587,7 @@
       </c>
       <c r="N123" s="2"/>
       <c r="O123" s="2"/>
-      <c r="P123" s="2"/>
+      <c r="P123" s="6"/>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
@@ -4556,7 +4615,7 @@
       </c>
       <c r="N124" s="2"/>
       <c r="O124" s="2"/>
-      <c r="P124" s="2"/>
+      <c r="P124" s="6"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
@@ -4584,7 +4643,7 @@
       </c>
       <c r="N125" s="2"/>
       <c r="O125" s="2"/>
-      <c r="P125" s="2"/>
+      <c r="P125" s="6"/>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
@@ -4612,7 +4671,7 @@
       </c>
       <c r="N126" s="2"/>
       <c r="O126" s="2"/>
-      <c r="P126" s="2"/>
+      <c r="P126" s="6"/>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
@@ -4640,7 +4699,7 @@
       </c>
       <c r="N127" s="2"/>
       <c r="O127" s="2"/>
-      <c r="P127" s="2"/>
+      <c r="P127" s="6"/>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
@@ -4668,7 +4727,7 @@
       </c>
       <c r="N128" s="2"/>
       <c r="O128" s="2"/>
-      <c r="P128" s="2"/>
+      <c r="P128" s="6"/>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
@@ -4696,7 +4755,7 @@
       </c>
       <c r="N129" s="2"/>
       <c r="O129" s="2"/>
-      <c r="P129" s="2"/>
+      <c r="P129" s="6"/>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
@@ -4724,7 +4783,7 @@
       </c>
       <c r="N130" s="2"/>
       <c r="O130" s="2"/>
-      <c r="P130" s="2"/>
+      <c r="P130" s="6"/>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
@@ -4752,7 +4811,7 @@
       </c>
       <c r="N131" s="2"/>
       <c r="O131" s="2"/>
-      <c r="P131" s="2"/>
+      <c r="P131" s="6"/>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
@@ -4780,7 +4839,7 @@
       </c>
       <c r="N132" s="2"/>
       <c r="O132" s="2"/>
-      <c r="P132" s="2"/>
+      <c r="P132" s="6"/>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
@@ -4828,7 +4887,7 @@
       <c r="O133" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P133" s="3" t="s">
+      <c r="P133" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4858,7 +4917,7 @@
       </c>
       <c r="N134" s="2"/>
       <c r="O134" s="2"/>
-      <c r="P134" s="2"/>
+      <c r="P134" s="6"/>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
@@ -4886,7 +4945,7 @@
       </c>
       <c r="N135" s="2"/>
       <c r="O135" s="2"/>
-      <c r="P135" s="2"/>
+      <c r="P135" s="6"/>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
@@ -4914,7 +4973,7 @@
       </c>
       <c r="N136" s="2"/>
       <c r="O136" s="2"/>
-      <c r="P136" s="2"/>
+      <c r="P136" s="6"/>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
@@ -4942,7 +5001,7 @@
       </c>
       <c r="N137" s="2"/>
       <c r="O137" s="2"/>
-      <c r="P137" s="2"/>
+      <c r="P137" s="6"/>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
@@ -4970,7 +5029,7 @@
       </c>
       <c r="N138" s="2"/>
       <c r="O138" s="2"/>
-      <c r="P138" s="2"/>
+      <c r="P138" s="6"/>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
@@ -4998,7 +5057,7 @@
       </c>
       <c r="N139" s="2"/>
       <c r="O139" s="2"/>
-      <c r="P139" s="2"/>
+      <c r="P139" s="6"/>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
@@ -5026,7 +5085,7 @@
       </c>
       <c r="N140" s="2"/>
       <c r="O140" s="2"/>
-      <c r="P140" s="2"/>
+      <c r="P140" s="6"/>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
@@ -5054,7 +5113,7 @@
       </c>
       <c r="N141" s="2"/>
       <c r="O141" s="2"/>
-      <c r="P141" s="2"/>
+      <c r="P141" s="6"/>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
@@ -5082,7 +5141,7 @@
       </c>
       <c r="N142" s="2"/>
       <c r="O142" s="2"/>
-      <c r="P142" s="2"/>
+      <c r="P142" s="6"/>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
@@ -5110,7 +5169,7 @@
       </c>
       <c r="N143" s="2"/>
       <c r="O143" s="2"/>
-      <c r="P143" s="2"/>
+      <c r="P143" s="6"/>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
@@ -5138,7 +5197,7 @@
       </c>
       <c r="N144" s="2"/>
       <c r="O144" s="2"/>
-      <c r="P144" s="2"/>
+      <c r="P144" s="6"/>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
@@ -5166,7 +5225,7 @@
       </c>
       <c r="N145" s="2"/>
       <c r="O145" s="2"/>
-      <c r="P145" s="2"/>
+      <c r="P145" s="6"/>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
@@ -5194,7 +5253,7 @@
       </c>
       <c r="N146" s="2"/>
       <c r="O146" s="2"/>
-      <c r="P146" s="2"/>
+      <c r="P146" s="6"/>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
@@ -5222,7 +5281,7 @@
       </c>
       <c r="N147" s="2"/>
       <c r="O147" s="2"/>
-      <c r="P147" s="2"/>
+      <c r="P147" s="6"/>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
@@ -5250,7 +5309,7 @@
       </c>
       <c r="N148" s="2"/>
       <c r="O148" s="2"/>
-      <c r="P148" s="2"/>
+      <c r="P148" s="6"/>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
@@ -5278,7 +5337,7 @@
       </c>
       <c r="N149" s="2"/>
       <c r="O149" s="2"/>
-      <c r="P149" s="2"/>
+      <c r="P149" s="6"/>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
@@ -5306,7 +5365,7 @@
       </c>
       <c r="N150" s="2"/>
       <c r="O150" s="2"/>
-      <c r="P150" s="2"/>
+      <c r="P150" s="6"/>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
@@ -5334,7 +5393,7 @@
       </c>
       <c r="N151" s="2"/>
       <c r="O151" s="2"/>
-      <c r="P151" s="2"/>
+      <c r="P151" s="6"/>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
@@ -5362,7 +5421,7 @@
       </c>
       <c r="N152" s="2"/>
       <c r="O152" s="2"/>
-      <c r="P152" s="2"/>
+      <c r="P152" s="6"/>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
@@ -5390,7 +5449,7 @@
       </c>
       <c r="N153" s="2"/>
       <c r="O153" s="2"/>
-      <c r="P153" s="2"/>
+      <c r="P153" s="6"/>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
@@ -5418,7 +5477,7 @@
       </c>
       <c r="N154" s="2"/>
       <c r="O154" s="2"/>
-      <c r="P154" s="2"/>
+      <c r="P154" s="6"/>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
@@ -5446,7 +5505,7 @@
       </c>
       <c r="N155" s="2"/>
       <c r="O155" s="2"/>
-      <c r="P155" s="2"/>
+      <c r="P155" s="6"/>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
@@ -5474,7 +5533,7 @@
       </c>
       <c r="N156" s="2"/>
       <c r="O156" s="2"/>
-      <c r="P156" s="2"/>
+      <c r="P156" s="6"/>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
@@ -5502,7 +5561,7 @@
       </c>
       <c r="N157" s="2"/>
       <c r="O157" s="2"/>
-      <c r="P157" s="2"/>
+      <c r="P157" s="6"/>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
@@ -5530,7 +5589,7 @@
       </c>
       <c r="N158" s="2"/>
       <c r="O158" s="2"/>
-      <c r="P158" s="2"/>
+      <c r="P158" s="6"/>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
@@ -5558,7 +5617,7 @@
       </c>
       <c r="N159" s="2"/>
       <c r="O159" s="2"/>
-      <c r="P159" s="2"/>
+      <c r="P159" s="6"/>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
@@ -5586,7 +5645,7 @@
       </c>
       <c r="N160" s="2"/>
       <c r="O160" s="2"/>
-      <c r="P160" s="2"/>
+      <c r="P160" s="6"/>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
@@ -5614,7 +5673,7 @@
       </c>
       <c r="N161" s="2"/>
       <c r="O161" s="2"/>
-      <c r="P161" s="2"/>
+      <c r="P161" s="6"/>
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
@@ -5642,7 +5701,7 @@
       </c>
       <c r="N162" s="2"/>
       <c r="O162" s="2"/>
-      <c r="P162" s="2"/>
+      <c r="P162" s="6"/>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
@@ -5670,7 +5729,7 @@
       </c>
       <c r="N163" s="2"/>
       <c r="O163" s="2"/>
-      <c r="P163" s="2"/>
+      <c r="P163" s="6"/>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
@@ -5698,7 +5757,7 @@
       </c>
       <c r="N164" s="2"/>
       <c r="O164" s="2"/>
-      <c r="P164" s="2"/>
+      <c r="P164" s="6"/>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
@@ -5726,7 +5785,7 @@
       </c>
       <c r="N165" s="2"/>
       <c r="O165" s="2"/>
-      <c r="P165" s="2"/>
+      <c r="P165" s="6"/>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
@@ -5774,7 +5833,7 @@
       <c r="O166" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P166" s="3" t="s">
+      <c r="P166" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5804,7 +5863,7 @@
       </c>
       <c r="N167" s="2"/>
       <c r="O167" s="2"/>
-      <c r="P167" s="2"/>
+      <c r="P167" s="6"/>
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
@@ -5832,7 +5891,7 @@
       </c>
       <c r="N168" s="2"/>
       <c r="O168" s="2"/>
-      <c r="P168" s="2"/>
+      <c r="P168" s="6"/>
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
@@ -5860,7 +5919,7 @@
       </c>
       <c r="N169" s="2"/>
       <c r="O169" s="2"/>
-      <c r="P169" s="2"/>
+      <c r="P169" s="6"/>
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
@@ -5888,7 +5947,7 @@
       </c>
       <c r="N170" s="2"/>
       <c r="O170" s="2"/>
-      <c r="P170" s="2"/>
+      <c r="P170" s="6"/>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
@@ -5916,7 +5975,7 @@
       </c>
       <c r="N171" s="2"/>
       <c r="O171" s="2"/>
-      <c r="P171" s="2"/>
+      <c r="P171" s="6"/>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
@@ -5944,7 +6003,7 @@
       </c>
       <c r="N172" s="2"/>
       <c r="O172" s="2"/>
-      <c r="P172" s="2"/>
+      <c r="P172" s="6"/>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
@@ -5972,7 +6031,7 @@
       </c>
       <c r="N173" s="2"/>
       <c r="O173" s="2"/>
-      <c r="P173" s="2"/>
+      <c r="P173" s="6"/>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
@@ -6000,7 +6059,7 @@
       </c>
       <c r="N174" s="2"/>
       <c r="O174" s="2"/>
-      <c r="P174" s="2"/>
+      <c r="P174" s="6"/>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
@@ -6028,7 +6087,7 @@
       </c>
       <c r="N175" s="2"/>
       <c r="O175" s="2"/>
-      <c r="P175" s="2"/>
+      <c r="P175" s="6"/>
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
@@ -6056,7 +6115,7 @@
       </c>
       <c r="N176" s="2"/>
       <c r="O176" s="2"/>
-      <c r="P176" s="2"/>
+      <c r="P176" s="6"/>
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
@@ -6084,7 +6143,7 @@
       </c>
       <c r="N177" s="2"/>
       <c r="O177" s="2"/>
-      <c r="P177" s="2"/>
+      <c r="P177" s="6"/>
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
@@ -6112,7 +6171,7 @@
       </c>
       <c r="N178" s="2"/>
       <c r="O178" s="2"/>
-      <c r="P178" s="2"/>
+      <c r="P178" s="6"/>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
@@ -6140,7 +6199,7 @@
       </c>
       <c r="N179" s="2"/>
       <c r="O179" s="2"/>
-      <c r="P179" s="2"/>
+      <c r="P179" s="6"/>
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
@@ -6168,7 +6227,7 @@
       </c>
       <c r="N180" s="2"/>
       <c r="O180" s="2"/>
-      <c r="P180" s="2"/>
+      <c r="P180" s="6"/>
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
@@ -6196,7 +6255,7 @@
       </c>
       <c r="N181" s="2"/>
       <c r="O181" s="2"/>
-      <c r="P181" s="2"/>
+      <c r="P181" s="6"/>
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
@@ -6224,7 +6283,7 @@
       </c>
       <c r="N182" s="2"/>
       <c r="O182" s="2"/>
-      <c r="P182" s="2"/>
+      <c r="P182" s="6"/>
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
@@ -6252,7 +6311,7 @@
       </c>
       <c r="N183" s="2"/>
       <c r="O183" s="2"/>
-      <c r="P183" s="2"/>
+      <c r="P183" s="6"/>
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
@@ -6280,7 +6339,7 @@
       </c>
       <c r="N184" s="2"/>
       <c r="O184" s="2"/>
-      <c r="P184" s="2"/>
+      <c r="P184" s="6"/>
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
@@ -6308,7 +6367,7 @@
       </c>
       <c r="N185" s="2"/>
       <c r="O185" s="2"/>
-      <c r="P185" s="2"/>
+      <c r="P185" s="6"/>
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
@@ -6336,7 +6395,7 @@
       </c>
       <c r="N186" s="2"/>
       <c r="O186" s="2"/>
-      <c r="P186" s="2"/>
+      <c r="P186" s="6"/>
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
@@ -6364,7 +6423,7 @@
       </c>
       <c r="N187" s="2"/>
       <c r="O187" s="2"/>
-      <c r="P187" s="2"/>
+      <c r="P187" s="6"/>
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
@@ -6392,7 +6451,7 @@
       </c>
       <c r="N188" s="2"/>
       <c r="O188" s="2"/>
-      <c r="P188" s="2"/>
+      <c r="P188" s="6"/>
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
@@ -6420,7 +6479,7 @@
       </c>
       <c r="N189" s="2"/>
       <c r="O189" s="2"/>
-      <c r="P189" s="2"/>
+      <c r="P189" s="6"/>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
@@ -6448,7 +6507,7 @@
       </c>
       <c r="N190" s="2"/>
       <c r="O190" s="2"/>
-      <c r="P190" s="2"/>
+      <c r="P190" s="6"/>
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
@@ -6476,7 +6535,7 @@
       </c>
       <c r="N191" s="2"/>
       <c r="O191" s="2"/>
-      <c r="P191" s="2"/>
+      <c r="P191" s="6"/>
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
@@ -6504,7 +6563,7 @@
       </c>
       <c r="N192" s="2"/>
       <c r="O192" s="2"/>
-      <c r="P192" s="2"/>
+      <c r="P192" s="6"/>
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
@@ -6532,7 +6591,7 @@
       </c>
       <c r="N193" s="2"/>
       <c r="O193" s="2"/>
-      <c r="P193" s="2"/>
+      <c r="P193" s="6"/>
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
@@ -6560,7 +6619,7 @@
       </c>
       <c r="N194" s="2"/>
       <c r="O194" s="2"/>
-      <c r="P194" s="2"/>
+      <c r="P194" s="6"/>
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
@@ -6588,7 +6647,7 @@
       </c>
       <c r="N195" s="2"/>
       <c r="O195" s="2"/>
-      <c r="P195" s="2"/>
+      <c r="P195" s="6"/>
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
@@ -6616,7 +6675,7 @@
       </c>
       <c r="N196" s="2"/>
       <c r="O196" s="2"/>
-      <c r="P196" s="2"/>
+      <c r="P196" s="6"/>
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
@@ -6644,7 +6703,7 @@
       </c>
       <c r="N197" s="2"/>
       <c r="O197" s="2"/>
-      <c r="P197" s="2"/>
+      <c r="P197" s="6"/>
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
@@ -6672,7 +6731,7 @@
       </c>
       <c r="N198" s="2"/>
       <c r="O198" s="2"/>
-      <c r="P198" s="2"/>
+      <c r="P198" s="6"/>
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
@@ -6720,7 +6779,7 @@
       <c r="O199" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P199" s="3" t="s">
+      <c r="P199" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -6750,7 +6809,7 @@
       </c>
       <c r="N200" s="2"/>
       <c r="O200" s="2"/>
-      <c r="P200" s="2"/>
+      <c r="P200" s="6"/>
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
@@ -6778,7 +6837,7 @@
       </c>
       <c r="N201" s="2"/>
       <c r="O201" s="2"/>
-      <c r="P201" s="2"/>
+      <c r="P201" s="6"/>
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
@@ -6806,7 +6865,7 @@
       </c>
       <c r="N202" s="2"/>
       <c r="O202" s="2"/>
-      <c r="P202" s="2"/>
+      <c r="P202" s="6"/>
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
@@ -6834,7 +6893,7 @@
       </c>
       <c r="N203" s="2"/>
       <c r="O203" s="2"/>
-      <c r="P203" s="2"/>
+      <c r="P203" s="6"/>
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
@@ -6862,7 +6921,7 @@
       </c>
       <c r="N204" s="2"/>
       <c r="O204" s="2"/>
-      <c r="P204" s="2"/>
+      <c r="P204" s="6"/>
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
@@ -6890,7 +6949,7 @@
       </c>
       <c r="N205" s="2"/>
       <c r="O205" s="2"/>
-      <c r="P205" s="2"/>
+      <c r="P205" s="6"/>
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
@@ -6918,7 +6977,7 @@
       </c>
       <c r="N206" s="2"/>
       <c r="O206" s="2"/>
-      <c r="P206" s="2"/>
+      <c r="P206" s="6"/>
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A207" s="2">
@@ -6946,7 +7005,7 @@
       </c>
       <c r="N207" s="2"/>
       <c r="O207" s="2"/>
-      <c r="P207" s="2"/>
+      <c r="P207" s="6"/>
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
@@ -6974,7 +7033,7 @@
       </c>
       <c r="N208" s="2"/>
       <c r="O208" s="2"/>
-      <c r="P208" s="2"/>
+      <c r="P208" s="6"/>
     </row>
     <row r="209" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
@@ -7002,7 +7061,7 @@
       </c>
       <c r="N209" s="2"/>
       <c r="O209" s="2"/>
-      <c r="P209" s="2"/>
+      <c r="P209" s="6"/>
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
@@ -7030,7 +7089,7 @@
       </c>
       <c r="N210" s="2"/>
       <c r="O210" s="2"/>
-      <c r="P210" s="2"/>
+      <c r="P210" s="6"/>
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
@@ -7058,7 +7117,7 @@
       </c>
       <c r="N211" s="2"/>
       <c r="O211" s="2"/>
-      <c r="P211" s="2"/>
+      <c r="P211" s="6"/>
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
@@ -7086,7 +7145,7 @@
       </c>
       <c r="N212" s="2"/>
       <c r="O212" s="2"/>
-      <c r="P212" s="2"/>
+      <c r="P212" s="6"/>
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
@@ -7114,7 +7173,7 @@
       </c>
       <c r="N213" s="2"/>
       <c r="O213" s="2"/>
-      <c r="P213" s="2"/>
+      <c r="P213" s="6"/>
     </row>
     <row r="214" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
@@ -7142,7 +7201,7 @@
       </c>
       <c r="N214" s="2"/>
       <c r="O214" s="2"/>
-      <c r="P214" s="2"/>
+      <c r="P214" s="6"/>
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
@@ -7170,7 +7229,7 @@
       </c>
       <c r="N215" s="2"/>
       <c r="O215" s="2"/>
-      <c r="P215" s="2"/>
+      <c r="P215" s="6"/>
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
@@ -7198,7 +7257,7 @@
       </c>
       <c r="N216" s="2"/>
       <c r="O216" s="2"/>
-      <c r="P216" s="2"/>
+      <c r="P216" s="6"/>
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
@@ -7226,7 +7285,7 @@
       </c>
       <c r="N217" s="2"/>
       <c r="O217" s="2"/>
-      <c r="P217" s="2"/>
+      <c r="P217" s="6"/>
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
@@ -7254,7 +7313,7 @@
       </c>
       <c r="N218" s="2"/>
       <c r="O218" s="2"/>
-      <c r="P218" s="2"/>
+      <c r="P218" s="6"/>
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
@@ -7282,7 +7341,7 @@
       </c>
       <c r="N219" s="2"/>
       <c r="O219" s="2"/>
-      <c r="P219" s="2"/>
+      <c r="P219" s="6"/>
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
@@ -7310,7 +7369,7 @@
       </c>
       <c r="N220" s="2"/>
       <c r="O220" s="2"/>
-      <c r="P220" s="2"/>
+      <c r="P220" s="6"/>
     </row>
     <row r="221" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
@@ -7338,7 +7397,7 @@
       </c>
       <c r="N221" s="2"/>
       <c r="O221" s="2"/>
-      <c r="P221" s="2"/>
+      <c r="P221" s="6"/>
     </row>
     <row r="222" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
@@ -7366,7 +7425,7 @@
       </c>
       <c r="N222" s="2"/>
       <c r="O222" s="2"/>
-      <c r="P222" s="2"/>
+      <c r="P222" s="6"/>
     </row>
     <row r="223" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
@@ -7394,7 +7453,7 @@
       </c>
       <c r="N223" s="2"/>
       <c r="O223" s="2"/>
-      <c r="P223" s="2"/>
+      <c r="P223" s="6"/>
     </row>
     <row r="224" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
@@ -7422,7 +7481,7 @@
       </c>
       <c r="N224" s="2"/>
       <c r="O224" s="2"/>
-      <c r="P224" s="2"/>
+      <c r="P224" s="6"/>
     </row>
     <row r="225" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
@@ -7450,7 +7509,7 @@
       </c>
       <c r="N225" s="2"/>
       <c r="O225" s="2"/>
-      <c r="P225" s="2"/>
+      <c r="P225" s="6"/>
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
@@ -7478,7 +7537,7 @@
       </c>
       <c r="N226" s="2"/>
       <c r="O226" s="2"/>
-      <c r="P226" s="2"/>
+      <c r="P226" s="6"/>
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A227" s="2">
@@ -7506,7 +7565,7 @@
       </c>
       <c r="N227" s="2"/>
       <c r="O227" s="2"/>
-      <c r="P227" s="2"/>
+      <c r="P227" s="6"/>
     </row>
     <row r="228" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
@@ -7534,7 +7593,7 @@
       </c>
       <c r="N228" s="2"/>
       <c r="O228" s="2"/>
-      <c r="P228" s="2"/>
+      <c r="P228" s="6"/>
     </row>
     <row r="229" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A229" s="2">
@@ -7562,7 +7621,7 @@
       </c>
       <c r="N229" s="2"/>
       <c r="O229" s="2"/>
-      <c r="P229" s="2"/>
+      <c r="P229" s="6"/>
     </row>
     <row r="230" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
@@ -7590,7 +7649,7 @@
       </c>
       <c r="N230" s="2"/>
       <c r="O230" s="2"/>
-      <c r="P230" s="2"/>
+      <c r="P230" s="6"/>
     </row>
     <row r="231" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A231" s="2">
@@ -7618,7 +7677,7 @@
       </c>
       <c r="N231" s="2"/>
       <c r="O231" s="2"/>
-      <c r="P231" s="2"/>
+      <c r="P231" s="6"/>
     </row>
     <row r="232" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
@@ -7666,7 +7725,7 @@
       <c r="O232" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P232" s="3" t="s">
+      <c r="P232" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -7696,7 +7755,7 @@
       </c>
       <c r="N233" s="2"/>
       <c r="O233" s="2"/>
-      <c r="P233" s="2"/>
+      <c r="P233" s="6"/>
     </row>
     <row r="234" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A234" s="2">
@@ -7724,7 +7783,7 @@
       </c>
       <c r="N234" s="2"/>
       <c r="O234" s="2"/>
-      <c r="P234" s="2"/>
+      <c r="P234" s="6"/>
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A235" s="2">
@@ -7752,7 +7811,7 @@
       </c>
       <c r="N235" s="2"/>
       <c r="O235" s="2"/>
-      <c r="P235" s="2"/>
+      <c r="P235" s="6"/>
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A236" s="2">
@@ -7780,7 +7839,7 @@
       </c>
       <c r="N236" s="2"/>
       <c r="O236" s="2"/>
-      <c r="P236" s="2"/>
+      <c r="P236" s="6"/>
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A237" s="2">
@@ -7808,7 +7867,7 @@
       </c>
       <c r="N237" s="2"/>
       <c r="O237" s="2"/>
-      <c r="P237" s="2"/>
+      <c r="P237" s="6"/>
     </row>
     <row r="238" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A238" s="2">
@@ -7836,7 +7895,7 @@
       </c>
       <c r="N238" s="2"/>
       <c r="O238" s="2"/>
-      <c r="P238" s="2"/>
+      <c r="P238" s="6"/>
     </row>
     <row r="239" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A239" s="2">
@@ -7864,7 +7923,7 @@
       </c>
       <c r="N239" s="2"/>
       <c r="O239" s="2"/>
-      <c r="P239" s="2"/>
+      <c r="P239" s="6"/>
     </row>
     <row r="240" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A240" s="2">
@@ -7892,7 +7951,7 @@
       </c>
       <c r="N240" s="2"/>
       <c r="O240" s="2"/>
-      <c r="P240" s="2"/>
+      <c r="P240" s="6"/>
     </row>
     <row r="241" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A241" s="2">
@@ -7920,7 +7979,7 @@
       </c>
       <c r="N241" s="2"/>
       <c r="O241" s="2"/>
-      <c r="P241" s="2"/>
+      <c r="P241" s="6"/>
     </row>
     <row r="242" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A242" s="2">
@@ -7948,7 +8007,7 @@
       </c>
       <c r="N242" s="2"/>
       <c r="O242" s="2"/>
-      <c r="P242" s="2"/>
+      <c r="P242" s="6"/>
     </row>
     <row r="243" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A243" s="2">
@@ -7976,7 +8035,7 @@
       </c>
       <c r="N243" s="2"/>
       <c r="O243" s="2"/>
-      <c r="P243" s="2"/>
+      <c r="P243" s="6"/>
     </row>
     <row r="244" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A244" s="2">
@@ -8004,7 +8063,7 @@
       </c>
       <c r="N244" s="2"/>
       <c r="O244" s="2"/>
-      <c r="P244" s="2"/>
+      <c r="P244" s="6"/>
     </row>
     <row r="245" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A245" s="2">
@@ -8032,7 +8091,7 @@
       </c>
       <c r="N245" s="2"/>
       <c r="O245" s="2"/>
-      <c r="P245" s="2"/>
+      <c r="P245" s="6"/>
     </row>
     <row r="246" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A246" s="2">
@@ -8060,7 +8119,7 @@
       </c>
       <c r="N246" s="2"/>
       <c r="O246" s="2"/>
-      <c r="P246" s="2"/>
+      <c r="P246" s="6"/>
     </row>
     <row r="247" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A247" s="2">
@@ -8088,7 +8147,7 @@
       </c>
       <c r="N247" s="2"/>
       <c r="O247" s="2"/>
-      <c r="P247" s="2"/>
+      <c r="P247" s="6"/>
     </row>
     <row r="248" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A248" s="2">
@@ -8116,7 +8175,7 @@
       </c>
       <c r="N248" s="2"/>
       <c r="O248" s="2"/>
-      <c r="P248" s="2"/>
+      <c r="P248" s="6"/>
     </row>
     <row r="249" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A249" s="2">
@@ -8144,7 +8203,7 @@
       </c>
       <c r="N249" s="2"/>
       <c r="O249" s="2"/>
-      <c r="P249" s="2"/>
+      <c r="P249" s="6"/>
     </row>
     <row r="250" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A250" s="2">
@@ -8172,7 +8231,7 @@
       </c>
       <c r="N250" s="2"/>
       <c r="O250" s="2"/>
-      <c r="P250" s="2"/>
+      <c r="P250" s="6"/>
     </row>
     <row r="251" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A251" s="2">
@@ -8200,7 +8259,7 @@
       </c>
       <c r="N251" s="2"/>
       <c r="O251" s="2"/>
-      <c r="P251" s="2"/>
+      <c r="P251" s="6"/>
     </row>
     <row r="252" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A252" s="2">
@@ -8228,7 +8287,7 @@
       </c>
       <c r="N252" s="2"/>
       <c r="O252" s="2"/>
-      <c r="P252" s="2"/>
+      <c r="P252" s="6"/>
     </row>
     <row r="253" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A253" s="2">
@@ -8256,7 +8315,7 @@
       </c>
       <c r="N253" s="2"/>
       <c r="O253" s="2"/>
-      <c r="P253" s="2"/>
+      <c r="P253" s="6"/>
     </row>
     <row r="254" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A254" s="2">
@@ -8284,7 +8343,7 @@
       </c>
       <c r="N254" s="2"/>
       <c r="O254" s="2"/>
-      <c r="P254" s="2"/>
+      <c r="P254" s="6"/>
     </row>
     <row r="255" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A255" s="2">
@@ -8312,7 +8371,7 @@
       </c>
       <c r="N255" s="2"/>
       <c r="O255" s="2"/>
-      <c r="P255" s="2"/>
+      <c r="P255" s="6"/>
     </row>
     <row r="256" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A256" s="2">
@@ -8340,7 +8399,7 @@
       </c>
       <c r="N256" s="2"/>
       <c r="O256" s="2"/>
-      <c r="P256" s="2"/>
+      <c r="P256" s="6"/>
     </row>
     <row r="257" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A257" s="2">
@@ -8368,7 +8427,7 @@
       </c>
       <c r="N257" s="2"/>
       <c r="O257" s="2"/>
-      <c r="P257" s="2"/>
+      <c r="P257" s="6"/>
     </row>
     <row r="258" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A258" s="2">
@@ -8396,7 +8455,7 @@
       </c>
       <c r="N258" s="2"/>
       <c r="O258" s="2"/>
-      <c r="P258" s="2"/>
+      <c r="P258" s="6"/>
     </row>
     <row r="259" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A259" s="2">
@@ -8424,7 +8483,7 @@
       </c>
       <c r="N259" s="2"/>
       <c r="O259" s="2"/>
-      <c r="P259" s="2"/>
+      <c r="P259" s="6"/>
     </row>
     <row r="260" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A260" s="2">
@@ -8452,7 +8511,7 @@
       </c>
       <c r="N260" s="2"/>
       <c r="O260" s="2"/>
-      <c r="P260" s="2"/>
+      <c r="P260" s="6"/>
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A261" s="2">
@@ -8480,7 +8539,7 @@
       </c>
       <c r="N261" s="2"/>
       <c r="O261" s="2"/>
-      <c r="P261" s="2"/>
+      <c r="P261" s="6"/>
     </row>
     <row r="262" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A262" s="2">
@@ -8508,7 +8567,7 @@
       </c>
       <c r="N262" s="2"/>
       <c r="O262" s="2"/>
-      <c r="P262" s="2"/>
+      <c r="P262" s="6"/>
     </row>
     <row r="263" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A263" s="2">
@@ -8536,7 +8595,7 @@
       </c>
       <c r="N263" s="2"/>
       <c r="O263" s="2"/>
-      <c r="P263" s="2"/>
+      <c r="P263" s="6"/>
     </row>
     <row r="264" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A264" s="2">
@@ -8564,7 +8623,7 @@
       </c>
       <c r="N264" s="2"/>
       <c r="O264" s="2"/>
-      <c r="P264" s="2"/>
+      <c r="P264" s="6"/>
     </row>
     <row r="265" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
@@ -8612,7 +8671,7 @@
       <c r="O265" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P265" s="3" t="s">
+      <c r="P265" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -8642,7 +8701,7 @@
       </c>
       <c r="N266" s="2"/>
       <c r="O266" s="2"/>
-      <c r="P266" s="2"/>
+      <c r="P266" s="6"/>
     </row>
     <row r="267" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A267" s="2">
@@ -8670,7 +8729,7 @@
       </c>
       <c r="N267" s="2"/>
       <c r="O267" s="2"/>
-      <c r="P267" s="2"/>
+      <c r="P267" s="6"/>
     </row>
     <row r="268" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A268" s="2">
@@ -8698,7 +8757,7 @@
       </c>
       <c r="N268" s="2"/>
       <c r="O268" s="2"/>
-      <c r="P268" s="2"/>
+      <c r="P268" s="6"/>
     </row>
     <row r="269" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A269" s="2">
@@ -8726,7 +8785,7 @@
       </c>
       <c r="N269" s="2"/>
       <c r="O269" s="2"/>
-      <c r="P269" s="2"/>
+      <c r="P269" s="6"/>
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A270" s="2">
@@ -8754,7 +8813,7 @@
       </c>
       <c r="N270" s="2"/>
       <c r="O270" s="2"/>
-      <c r="P270" s="2"/>
+      <c r="P270" s="6"/>
     </row>
     <row r="271" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A271" s="2">
@@ -8782,7 +8841,7 @@
       </c>
       <c r="N271" s="2"/>
       <c r="O271" s="2"/>
-      <c r="P271" s="2"/>
+      <c r="P271" s="6"/>
     </row>
     <row r="272" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A272" s="2">
@@ -8810,7 +8869,7 @@
       </c>
       <c r="N272" s="2"/>
       <c r="O272" s="2"/>
-      <c r="P272" s="2"/>
+      <c r="P272" s="6"/>
     </row>
     <row r="273" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A273" s="2">
@@ -8838,7 +8897,7 @@
       </c>
       <c r="N273" s="2"/>
       <c r="O273" s="2"/>
-      <c r="P273" s="2"/>
+      <c r="P273" s="6"/>
     </row>
     <row r="274" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A274" s="2"/>
@@ -8856,7 +8915,7 @@
       <c r="M274" s="2"/>
       <c r="N274" s="2"/>
       <c r="O274" s="2"/>
-      <c r="P274" s="2"/>
+      <c r="P274" s="6"/>
     </row>
     <row r="275" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A275" s="2"/>
@@ -8874,7 +8933,7 @@
       <c r="M275" s="2"/>
       <c r="N275" s="2"/>
       <c r="O275" s="2"/>
-      <c r="P275" s="2"/>
+      <c r="P275" s="6"/>
     </row>
     <row r="276" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A276" s="2"/>
@@ -8892,7 +8951,7 @@
       <c r="M276" s="2"/>
       <c r="N276" s="2"/>
       <c r="O276" s="2"/>
-      <c r="P276" s="2"/>
+      <c r="P276" s="6"/>
     </row>
     <row r="277" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A277" s="2"/>
@@ -8910,7 +8969,7 @@
       <c r="M277" s="2"/>
       <c r="N277" s="2"/>
       <c r="O277" s="2"/>
-      <c r="P277" s="2"/>
+      <c r="P277" s="6"/>
     </row>
     <row r="278" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A278" s="2"/>
@@ -8928,7 +8987,7 @@
       <c r="M278" s="2"/>
       <c r="N278" s="2"/>
       <c r="O278" s="2"/>
-      <c r="P278" s="2"/>
+      <c r="P278" s="6"/>
     </row>
     <row r="279" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A279" s="2"/>
@@ -8946,7 +9005,7 @@
       <c r="M279" s="2"/>
       <c r="N279" s="2"/>
       <c r="O279" s="2"/>
-      <c r="P279" s="2"/>
+      <c r="P279" s="6"/>
     </row>
     <row r="280" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A280" s="2"/>
@@ -8964,7 +9023,7 @@
       <c r="M280" s="2"/>
       <c r="N280" s="2"/>
       <c r="O280" s="2"/>
-      <c r="P280" s="2"/>
+      <c r="P280" s="6"/>
     </row>
     <row r="281" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A281" s="2"/>
@@ -8982,7 +9041,7 @@
       <c r="M281" s="2"/>
       <c r="N281" s="2"/>
       <c r="O281" s="2"/>
-      <c r="P281" s="2"/>
+      <c r="P281" s="6"/>
     </row>
     <row r="282" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A282" s="2"/>
@@ -9000,7 +9059,7 @@
       <c r="M282" s="2"/>
       <c r="N282" s="2"/>
       <c r="O282" s="2"/>
-      <c r="P282" s="2"/>
+      <c r="P282" s="6"/>
     </row>
     <row r="283" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A283" s="2"/>
@@ -9018,7 +9077,7 @@
       <c r="M283" s="2"/>
       <c r="N283" s="2"/>
       <c r="O283" s="2"/>
-      <c r="P283" s="2"/>
+      <c r="P283" s="6"/>
     </row>
     <row r="284" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A284" s="2"/>
@@ -9036,7 +9095,7 @@
       <c r="M284" s="2"/>
       <c r="N284" s="2"/>
       <c r="O284" s="2"/>
-      <c r="P284" s="2"/>
+      <c r="P284" s="6"/>
     </row>
     <row r="285" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A285" s="2"/>
@@ -9054,7 +9113,7 @@
       <c r="M285" s="2"/>
       <c r="N285" s="2"/>
       <c r="O285" s="2"/>
-      <c r="P285" s="2"/>
+      <c r="P285" s="6"/>
     </row>
     <row r="286" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A286" s="2"/>
@@ -9072,7 +9131,7 @@
       <c r="M286" s="2"/>
       <c r="N286" s="2"/>
       <c r="O286" s="2"/>
-      <c r="P286" s="2"/>
+      <c r="P286" s="6"/>
     </row>
     <row r="287" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A287" s="2"/>
@@ -9090,7 +9149,7 @@
       <c r="M287" s="2"/>
       <c r="N287" s="2"/>
       <c r="O287" s="2"/>
-      <c r="P287" s="2"/>
+      <c r="P287" s="6"/>
     </row>
     <row r="288" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A288" s="2"/>
@@ -9108,9 +9167,9 @@
       <c r="M288" s="2"/>
       <c r="N288" s="2"/>
       <c r="O288" s="2"/>
-      <c r="P288" s="2"/>
-    </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P288" s="6"/>
+    </row>
+    <row r="289" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A289" s="2"/>
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
@@ -9126,9 +9185,9 @@
       <c r="M289" s="2"/>
       <c r="N289" s="2"/>
       <c r="O289" s="2"/>
-      <c r="P289" s="2"/>
-    </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P289" s="6"/>
+    </row>
+    <row r="290" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A290" s="2"/>
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
@@ -9144,9 +9203,9 @@
       <c r="M290" s="2"/>
       <c r="N290" s="2"/>
       <c r="O290" s="2"/>
-      <c r="P290" s="2"/>
-    </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P290" s="6"/>
+    </row>
+    <row r="291" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A291" s="2"/>
       <c r="B291" s="2"/>
       <c r="C291" s="2"/>
@@ -9162,9 +9221,9 @@
       <c r="M291" s="2"/>
       <c r="N291" s="2"/>
       <c r="O291" s="2"/>
-      <c r="P291" s="2"/>
-    </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P291" s="6"/>
+    </row>
+    <row r="292" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A292" s="2"/>
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
@@ -9180,9 +9239,9 @@
       <c r="M292" s="2"/>
       <c r="N292" s="2"/>
       <c r="O292" s="2"/>
-      <c r="P292" s="2"/>
-    </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P292" s="6"/>
+    </row>
+    <row r="293" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A293" s="2"/>
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
@@ -9198,9 +9257,9 @@
       <c r="M293" s="2"/>
       <c r="N293" s="2"/>
       <c r="O293" s="2"/>
-      <c r="P293" s="2"/>
-    </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P293" s="6"/>
+    </row>
+    <row r="294" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A294" s="2"/>
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
@@ -9216,9 +9275,9 @@
       <c r="M294" s="2"/>
       <c r="N294" s="2"/>
       <c r="O294" s="2"/>
-      <c r="P294" s="2"/>
-    </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P294" s="6"/>
+    </row>
+    <row r="295" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A295" s="2"/>
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
@@ -9234,9 +9293,9 @@
       <c r="M295" s="2"/>
       <c r="N295" s="2"/>
       <c r="O295" s="2"/>
-      <c r="P295" s="2"/>
-    </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P295" s="6"/>
+    </row>
+    <row r="296" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A296" s="2"/>
       <c r="B296" s="2"/>
       <c r="C296" s="2"/>
@@ -9252,9 +9311,9 @@
       <c r="M296" s="2"/>
       <c r="N296" s="2"/>
       <c r="O296" s="2"/>
-      <c r="P296" s="2"/>
-    </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P296" s="6"/>
+    </row>
+    <row r="297" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A297" s="2"/>
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
@@ -9270,7 +9329,12 @@
       <c r="M297" s="2"/>
       <c r="N297" s="2"/>
       <c r="O297" s="2"/>
-      <c r="P297" s="2"/>
+      <c r="P297" s="6"/>
+    </row>
+    <row r="298" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="O298" s="7"/>
+      <c r="P298" s="8"/>
+      <c r="Q298" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>